<commit_message>
kw, wilcoxon test with corrections implemented.
</commit_message>
<xml_diff>
--- a/utils/paper/ad_table.xlsx
+++ b/utils/paper/ad_table.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valenciaem/coding/pipelines/utils/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A8856A-7AFC-F440-ABD1-5CC7931222EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3281259-FF5E-984A-A0A5-D5D261936F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="3520" windowWidth="23040" windowHeight="16900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="3500" windowWidth="23040" windowHeight="16900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AD table_species" sheetId="1" r:id="rId1"/>
     <sheet name="Sens" sheetId="2" r:id="rId2"/>
     <sheet name="FPRA" sheetId="3" r:id="rId3"/>
+    <sheet name="AD_Tidy" sheetId="4" r:id="rId4"/>
+    <sheet name="Sens_Tidy" sheetId="5" r:id="rId5"/>
+    <sheet name="FPRA_Tidy" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,15 +38,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="32">
   <si>
     <t>CamiSim-S2</t>
   </si>
   <si>
     <t>NIST-MIX-B</t>
-  </si>
-  <si>
-    <t>N Samples</t>
   </si>
   <si>
     <t>Bmock12</t>
@@ -114,12 +114,37 @@
   <si>
     <t>One-to-One</t>
   </si>
+  <si>
+    <t>Community</t>
+  </si>
+  <si>
+    <t>p&lt;0.001*</t>
+  </si>
+  <si>
+    <t>p=0.13*</t>
+  </si>
+  <si>
+    <t>p=0.002*</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Avg Complexity</t>
+  </si>
+  <si>
+    <t>Avg Score</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="0.000000"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,6 +193,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -186,10 +226,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -216,6 +257,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -228,11 +278,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -537,103 +591,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="150" workbookViewId="0">
-      <selection sqref="A1:M14"/>
+    <sheetView zoomScale="111" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.83203125" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+    </row>
+    <row r="2" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="16"/>
+      <c r="N2" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-    </row>
-    <row r="2" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="10" t="s">
+      <c r="B4" t="s">
         <v>2</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" s="13"/>
-    </row>
-    <row r="3" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
       </c>
       <c r="C4" s="8">
         <v>1</v>
@@ -658,11 +717,15 @@
         <v>26.448399999999999</v>
       </c>
       <c r="M4" s="9"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="12"/>
+      <c r="N4" s="9">
+        <f>AVERAGE(D4,F4,H4,J4,L4)</f>
+        <v>20.241659999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="15"/>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="8">
         <v>1</v>
@@ -687,9 +750,13 @@
         <v>30.759599999999999</v>
       </c>
       <c r="M5" s="9"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="12"/>
+      <c r="N5" s="9">
+        <f t="shared" ref="N5:N15" si="0">AVERAGE(D5,F5,H5,J5,L5)</f>
+        <v>16.131119999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="15"/>
       <c r="B6" t="s">
         <v>0</v>
       </c>
@@ -716,11 +783,15 @@
         <v>25.8766</v>
       </c>
       <c r="M6" s="9"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
+      <c r="N6" s="9">
+        <f t="shared" si="0"/>
+        <v>9.0904599999999984</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="15"/>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="8">
         <v>1</v>
@@ -745,11 +816,15 @@
         <v>22.595300000000002</v>
       </c>
       <c r="M7" s="9"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="12"/>
+      <c r="N7" s="9">
+        <f t="shared" si="0"/>
+        <v>12.927879999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="15"/>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="8">
         <v>1</v>
@@ -774,9 +849,13 @@
         <v>19.242000000000001</v>
       </c>
       <c r="M8" s="9"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="12"/>
+      <c r="N8" s="9">
+        <f t="shared" si="0"/>
+        <v>10.204000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="15"/>
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -803,11 +882,15 @@
         <v>22.8751</v>
       </c>
       <c r="M9" s="9"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="12"/>
+      <c r="N9" s="9">
+        <f t="shared" si="0"/>
+        <v>14.59418</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="15"/>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" s="8">
         <v>1</v>
@@ -832,11 +915,15 @@
         <v>24.102599999999999</v>
       </c>
       <c r="M10" s="9"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="12"/>
+      <c r="N10" s="9">
+        <f t="shared" si="0"/>
+        <v>16.328479999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="15"/>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" s="8">
         <v>1</v>
@@ -861,13 +948,17 @@
         <v>21.115500000000001</v>
       </c>
       <c r="M11" s="9"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
-        <v>18</v>
+      <c r="N11" s="9">
+        <f t="shared" si="0"/>
+        <v>9.9015999999999984</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="15" t="s">
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="8">
         <v>5</v>
@@ -902,11 +993,15 @@
       <c r="M12" s="4">
         <v>0.11231954399999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="12"/>
+      <c r="N12" s="9">
+        <f t="shared" si="0"/>
+        <v>10.546428000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="15"/>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="8">
         <v>5</v>
@@ -941,11 +1036,15 @@
       <c r="M13" s="4">
         <v>0.21670798799999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="12"/>
+      <c r="N13" s="9">
+        <f t="shared" si="0"/>
+        <v>11.327043999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="15"/>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" s="8">
         <v>6</v>
@@ -980,23 +1079,60 @@
       <c r="M14" s="4">
         <v>0.26064468099999999</v>
       </c>
+      <c r="N14" s="9">
+        <f t="shared" si="0"/>
+        <v>12.963663334</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="9">
+        <f t="shared" ref="D15:L15" si="1">AVERAGE(D4:D14)</f>
+        <v>9.9879948481818186</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9">
+        <f t="shared" si="1"/>
+        <v>6.9986572727272724</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9">
+        <f t="shared" si="1"/>
+        <v>12.742581818181817</v>
+      </c>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9">
+        <f t="shared" si="1"/>
+        <v>12.757096970000003</v>
+      </c>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9">
+        <f t="shared" si="1"/>
+        <v>23.084812424545454</v>
+      </c>
+      <c r="N15" s="9"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B16" s="5"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="5"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="6"/>
+      <c r="B17" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A4:A11"/>
-    <mergeCell ref="A1:M1"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="L2:M2"/>
+    <mergeCell ref="A1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1005,109 +1141,114 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B923C69-C9BB-6B48-83C3-9A3CA5A7DD02}">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView zoomScale="118" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="6" customWidth="1"/>
+    <col min="14" max="14" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="1"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15" t="s">
+      <c r="G2" s="18"/>
+      <c r="H2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15" t="s">
+      <c r="I2" s="18"/>
+      <c r="J2" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15" t="s">
+      <c r="K2" s="18"/>
+      <c r="L2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" s="15"/>
-      <c r="N2" s="1"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M2" s="18"/>
+      <c r="N2" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="H3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="J3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="L3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N3" s="1"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
-        <v>25</v>
+      <c r="N3" s="7"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="16">
+        <v>2</v>
+      </c>
+      <c r="C4" s="12">
         <v>1</v>
       </c>
       <c r="D4" s="9">
@@ -1130,14 +1271,18 @@
         <v>9.0908999999999995</v>
       </c>
       <c r="M4" s="9"/>
-      <c r="N4" s="3"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
+      <c r="N4" s="9">
+        <f>AVERAGE(D4,F4,H4,J4,L4)</f>
+        <v>41.818179999999998</v>
+      </c>
+      <c r="O4" s="20"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="17"/>
       <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="16">
+        <v>7</v>
+      </c>
+      <c r="C5" s="12">
         <v>1</v>
       </c>
       <c r="D5" s="9">
@@ -1160,14 +1305,18 @@
         <v>86.842100000000002</v>
       </c>
       <c r="M5" s="9"/>
-      <c r="N5" s="3"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
+      <c r="N5" s="9">
+        <f t="shared" ref="N5:N14" si="0">AVERAGE(D5,F5,H5,J5,L5)</f>
+        <v>94.210520000000002</v>
+      </c>
+      <c r="O5" s="20"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="17"/>
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="12">
         <v>1</v>
       </c>
       <c r="D6" s="9">
@@ -1190,14 +1339,18 @@
         <v>80.952399999999997</v>
       </c>
       <c r="M6" s="9"/>
-      <c r="N6" s="3"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
+      <c r="N6" s="9">
+        <f t="shared" si="0"/>
+        <v>95.238100000000003</v>
+      </c>
+      <c r="O6" s="20"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="17"/>
       <c r="B7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="16">
+        <v>4</v>
+      </c>
+      <c r="C7" s="12">
         <v>1</v>
       </c>
       <c r="D7" s="9">
@@ -1220,14 +1373,18 @@
         <v>85.714299999999994</v>
       </c>
       <c r="M7" s="9"/>
-      <c r="N7" s="3"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
+      <c r="N7" s="9">
+        <f t="shared" si="0"/>
+        <v>91.42855999999999</v>
+      </c>
+      <c r="O7" s="20"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="17"/>
       <c r="B8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="16">
+        <v>8</v>
+      </c>
+      <c r="C8" s="12">
         <v>1</v>
       </c>
       <c r="D8" s="9">
@@ -1250,14 +1407,18 @@
         <v>90.909099999999995</v>
       </c>
       <c r="M8" s="9"/>
-      <c r="N8" s="3"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
+      <c r="N8" s="9">
+        <f t="shared" si="0"/>
+        <v>87.272739999999999</v>
+      </c>
+      <c r="O8" s="20"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="17"/>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="12">
         <v>1</v>
       </c>
       <c r="D9" s="9">
@@ -1280,14 +1441,18 @@
         <v>90.909099999999995</v>
       </c>
       <c r="M9" s="9"/>
-      <c r="N9" s="3"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
+      <c r="N9" s="9">
+        <f t="shared" si="0"/>
+        <v>83.636380000000003</v>
+      </c>
+      <c r="O9" s="20"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="17"/>
       <c r="B10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="16">
+        <v>3</v>
+      </c>
+      <c r="C10" s="12">
         <v>1</v>
       </c>
       <c r="D10" s="9">
@@ -1310,14 +1475,18 @@
         <v>81.818200000000004</v>
       </c>
       <c r="M10" s="9"/>
-      <c r="N10" s="3"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
+      <c r="N10" s="9">
+        <f t="shared" si="0"/>
+        <v>80.000019999999992</v>
+      </c>
+      <c r="O10" s="20"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="17"/>
       <c r="B11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="16">
+        <v>6</v>
+      </c>
+      <c r="C11" s="12">
         <v>1</v>
       </c>
       <c r="D11" s="9">
@@ -1340,16 +1509,20 @@
         <v>81.818200000000004</v>
       </c>
       <c r="M11" s="9"/>
-      <c r="N11" s="3"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="14" t="s">
-        <v>18</v>
+      <c r="N11" s="9">
+        <f t="shared" si="0"/>
+        <v>81.818200000000004</v>
+      </c>
+      <c r="O11" s="20"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="16">
+        <v>22</v>
+      </c>
+      <c r="C12" s="12">
         <v>5</v>
       </c>
       <c r="D12" s="9">
@@ -1382,14 +1555,18 @@
       <c r="M12" s="9">
         <v>0</v>
       </c>
-      <c r="N12" s="3"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
+      <c r="N12" s="9">
+        <f t="shared" si="0"/>
+        <v>94.526312000000004</v>
+      </c>
+      <c r="O12" s="20"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="17"/>
       <c r="B13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="16">
+        <v>21</v>
+      </c>
+      <c r="C13" s="12">
         <v>5</v>
       </c>
       <c r="D13" s="9">
@@ -1422,14 +1599,18 @@
       <c r="M13" s="9">
         <v>0</v>
       </c>
-      <c r="N13" s="3"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
+      <c r="N13" s="9">
+        <f t="shared" si="0"/>
+        <v>95.789460000000005</v>
+      </c>
+      <c r="O13" s="20"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="17"/>
       <c r="B14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="16">
+        <v>9</v>
+      </c>
+      <c r="C14" s="12">
         <v>6</v>
       </c>
       <c r="D14" s="9">
@@ -1462,18 +1643,62 @@
       <c r="M14" s="9">
         <v>0</v>
       </c>
-      <c r="N14" s="3"/>
+      <c r="N14" s="9">
+        <f t="shared" si="0"/>
+        <v>91.578940000000017</v>
+      </c>
+      <c r="O14" s="20"/>
+    </row>
+    <row r="15" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="21">
+        <f>AVERAGE(D4:D14)</f>
+        <v>79.649545454545461</v>
+      </c>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21">
+        <f>AVERAGE(F4:F14)</f>
+        <v>85.085654545454545</v>
+      </c>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21">
+        <f>AVERAGE(H4:H14)</f>
+        <v>88.271923636363638</v>
+      </c>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21">
+        <f>AVERAGE(J4:J14)</f>
+        <v>91.931272727272727</v>
+      </c>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21">
+        <f>AVERAGE(L4:L14)</f>
+        <v>81.114972727272729</v>
+      </c>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="10"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D17" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A4:A11"/>
     <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A1:M1"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="L2:M2"/>
+    <mergeCell ref="A1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1481,100 +1706,110 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8632E733-9369-9C4A-92F9-C345ACE74E55}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="6.1640625" customWidth="1"/>
+    <col min="14" max="14" width="14.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15" t="s">
+      <c r="G2" s="18"/>
+      <c r="H2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15" t="s">
+      <c r="I2" s="18"/>
+      <c r="J2" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15" t="s">
+      <c r="K2" s="18"/>
+      <c r="L2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" s="15"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M2" s="18"/>
+      <c r="N2" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="H3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="J3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="L3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
-        <v>25</v>
+      <c r="N3" s="7"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="11">
         <v>1</v>
@@ -1599,11 +1834,15 @@
         <v>11.964700000000001</v>
       </c>
       <c r="M4" s="4"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
+      <c r="N4" s="9">
+        <f>AVERAGE(D4,F4,H4,J4,L4)</f>
+        <v>23.981939999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="17"/>
       <c r="B5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="11">
         <v>1</v>
@@ -1628,9 +1867,13 @@
         <v>8.5091000000000001</v>
       </c>
       <c r="M5" s="4"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
+      <c r="N5" s="9">
+        <f t="shared" ref="N5:N14" si="0">AVERAGE(D5,F5,H5,J5,L5)</f>
+        <v>3.1148400000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="17"/>
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1657,11 +1900,15 @@
         <v>30.666799999999999</v>
       </c>
       <c r="M6" s="4"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
+      <c r="N6" s="9">
+        <f t="shared" si="0"/>
+        <v>7.7351000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="17"/>
       <c r="B7" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="11">
         <v>1</v>
@@ -1686,11 +1933,15 @@
         <v>26.4802</v>
       </c>
       <c r="M7" s="4"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
+      <c r="N7" s="9">
+        <f t="shared" si="0"/>
+        <v>6.10304</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="17"/>
       <c r="B8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="11">
         <v>1</v>
@@ -1715,9 +1966,13 @@
         <v>30.915199999999999</v>
       </c>
       <c r="M8" s="4"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
+      <c r="N8" s="9">
+        <f t="shared" si="0"/>
+        <v>6.4983400000000007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="17"/>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
@@ -1744,11 +1999,15 @@
         <v>31.056799999999999</v>
       </c>
       <c r="M9" s="4"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
+      <c r="N9" s="9">
+        <f t="shared" si="0"/>
+        <v>8.7676800000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="17"/>
       <c r="B10" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" s="11">
         <v>1</v>
@@ -1773,11 +2032,15 @@
         <v>69.168199999999999</v>
       </c>
       <c r="M10" s="4"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
+      <c r="N10" s="9">
+        <f t="shared" si="0"/>
+        <v>33.005960000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="17"/>
       <c r="B11" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" s="11">
         <v>1</v>
@@ -1802,13 +2065,17 @@
         <v>13.194800000000001</v>
       </c>
       <c r="M11" s="4"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="14" t="s">
-        <v>18</v>
+      <c r="N11" s="9">
+        <f t="shared" si="0"/>
+        <v>2.7255799999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="11">
         <v>5</v>
@@ -1843,11 +2110,15 @@
       <c r="M12" s="9">
         <v>0.20599831795429799</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
+      <c r="N12" s="9">
+        <f t="shared" si="0"/>
+        <v>5.9168199999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="17"/>
       <c r="B13" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="11">
         <v>5</v>
@@ -1882,11 +2153,15 @@
       <c r="M13" s="9">
         <v>0.307409954295563</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
+      <c r="N13" s="9">
+        <f t="shared" si="0"/>
+        <v>11.014943999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="17"/>
       <c r="B14" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" s="11">
         <v>6</v>
@@ -1920,19 +2195,989 @@
       </c>
       <c r="M14" s="9">
         <v>0.24861157991265601</v>
+      </c>
+      <c r="N14" s="9">
+        <f t="shared" si="0"/>
+        <v>14.613239999999985</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="9">
+        <f>AVERAGE(D4:D14)</f>
+        <v>6.0325281818181802</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9">
+        <f t="shared" ref="F15:L15" si="1">AVERAGE(F4:F14)</f>
+        <v>5.6327378787878777</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9">
+        <f t="shared" si="1"/>
+        <v>8.8529906060606063</v>
+      </c>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9">
+        <f t="shared" si="1"/>
+        <v>8.5413666666666632</v>
+      </c>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9">
+        <f t="shared" si="1"/>
+        <v>27.066505757575758</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A4:A11"/>
     <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A1:M1"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="L2:M2"/>
+    <mergeCell ref="A1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F8738BA-7DB3-6C48-8963-B76731A2339F}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="9">
+        <f>'AD table_species'!D4</f>
+        <v>16.617999999999999</v>
+      </c>
+      <c r="C2" s="9">
+        <f>'AD table_species'!F4</f>
+        <v>11.3065</v>
+      </c>
+      <c r="D2" s="9">
+        <f>'AD table_species'!H4</f>
+        <v>22.368099999999998</v>
+      </c>
+      <c r="E2" s="9">
+        <f>'AD table_species'!J4</f>
+        <v>24.467300000000002</v>
+      </c>
+      <c r="F2" s="9">
+        <f>'AD table_species'!L4</f>
+        <v>26.448399999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="9">
+        <f>'AD table_species'!D5</f>
+        <v>8.6188000000000002</v>
+      </c>
+      <c r="C3" s="9">
+        <f>'AD table_species'!F5</f>
+        <v>12.764699999999999</v>
+      </c>
+      <c r="D3" s="9">
+        <f>'AD table_species'!H5</f>
+        <v>15.036099999999999</v>
+      </c>
+      <c r="E3" s="9">
+        <f>'AD table_species'!J5</f>
+        <v>13.4764</v>
+      </c>
+      <c r="F3" s="9">
+        <f>'AD table_species'!L5</f>
+        <v>30.759599999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="9">
+        <f>'AD table_species'!D6</f>
+        <v>1.2307999999999999</v>
+      </c>
+      <c r="C4" s="9">
+        <f>'AD table_species'!F6</f>
+        <v>7.1138000000000003</v>
+      </c>
+      <c r="D4" s="9">
+        <f>'AD table_species'!H6</f>
+        <v>4.8525</v>
+      </c>
+      <c r="E4" s="9">
+        <f>'AD table_species'!J6</f>
+        <v>6.3785999999999996</v>
+      </c>
+      <c r="F4" s="9">
+        <f>'AD table_species'!L6</f>
+        <v>25.8766</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9">
+        <f>'AD table_species'!D7</f>
+        <v>10.182600000000001</v>
+      </c>
+      <c r="C5" s="9">
+        <f>'AD table_species'!F7</f>
+        <v>8.9445999999999994</v>
+      </c>
+      <c r="D5" s="9">
+        <f>'AD table_species'!H7</f>
+        <v>12.2531</v>
+      </c>
+      <c r="E5" s="9">
+        <f>'AD table_species'!J7</f>
+        <v>10.6638</v>
+      </c>
+      <c r="F5" s="9">
+        <f>'AD table_species'!L7</f>
+        <v>22.595300000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="9">
+        <f>'AD table_species'!D8</f>
+        <v>9.5852000000000004</v>
+      </c>
+      <c r="C6" s="9">
+        <f>'AD table_species'!F8</f>
+        <v>2.8426</v>
+      </c>
+      <c r="D6" s="9">
+        <f>'AD table_species'!H8</f>
+        <v>12.3527</v>
+      </c>
+      <c r="E6" s="9">
+        <f>'AD table_species'!J8</f>
+        <v>6.9974999999999996</v>
+      </c>
+      <c r="F6" s="9">
+        <f>'AD table_species'!L8</f>
+        <v>19.242000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="9">
+        <f>'AD table_species'!D9</f>
+        <v>13.652200000000001</v>
+      </c>
+      <c r="C7" s="9">
+        <f>'AD table_species'!F9</f>
+        <v>9.8140000000000001</v>
+      </c>
+      <c r="D7" s="9">
+        <f>'AD table_species'!H9</f>
+        <v>13.5504</v>
+      </c>
+      <c r="E7" s="9">
+        <f>'AD table_species'!J9</f>
+        <v>13.0792</v>
+      </c>
+      <c r="F7" s="9">
+        <f>'AD table_species'!L9</f>
+        <v>22.8751</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="9">
+        <f>'AD table_species'!D10</f>
+        <v>14.108700000000001</v>
+      </c>
+      <c r="C8" s="9">
+        <f>'AD table_species'!F10</f>
+        <v>11.569000000000001</v>
+      </c>
+      <c r="D8" s="9">
+        <f>'AD table_species'!H10</f>
+        <v>17.1601</v>
+      </c>
+      <c r="E8" s="9">
+        <f>'AD table_species'!J10</f>
+        <v>14.702</v>
+      </c>
+      <c r="F8" s="9">
+        <f>'AD table_species'!L10</f>
+        <v>24.102599999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="9">
+        <f>'AD table_species'!D11</f>
+        <v>4.1345000000000001</v>
+      </c>
+      <c r="C9" s="9">
+        <f>'AD table_species'!F11</f>
+        <v>4.1097999999999999</v>
+      </c>
+      <c r="D9" s="9">
+        <f>'AD table_species'!H11</f>
+        <v>11.2166</v>
+      </c>
+      <c r="E9" s="9">
+        <f>'AD table_species'!J11</f>
+        <v>8.9315999999999995</v>
+      </c>
+      <c r="F9" s="9">
+        <f>'AD table_species'!L11</f>
+        <v>21.115500000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="9">
+        <f>'AD table_species'!D12</f>
+        <v>8.4025200000000009</v>
+      </c>
+      <c r="C10" s="9">
+        <f>'AD table_species'!F12</f>
+        <v>2.71252</v>
+      </c>
+      <c r="D10" s="9">
+        <f>'AD table_species'!H12</f>
+        <v>12.795640000000001</v>
+      </c>
+      <c r="E10" s="9">
+        <f>'AD table_species'!J12</f>
+        <v>12.436959999999999</v>
+      </c>
+      <c r="F10" s="9">
+        <f>'AD table_species'!L12</f>
+        <v>16.384499999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="9">
+        <f>'AD table_species'!D13</f>
+        <v>8.7674400000000006</v>
+      </c>
+      <c r="C11" s="9">
+        <f>'AD table_species'!F13</f>
+        <v>1.99916</v>
+      </c>
+      <c r="D11" s="9">
+        <f>'AD table_species'!H13</f>
+        <v>10.42296</v>
+      </c>
+      <c r="E11" s="9">
+        <f>'AD table_species'!J13</f>
+        <v>14.81574</v>
+      </c>
+      <c r="F11" s="9">
+        <f>'AD table_species'!L13</f>
+        <v>20.629919999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="9">
+        <f>'AD table_species'!D14</f>
+        <v>14.567183330000001</v>
+      </c>
+      <c r="C12" s="9">
+        <f>'AD table_species'!F14</f>
+        <v>3.8085499999999999</v>
+      </c>
+      <c r="D12" s="9">
+        <f>'AD table_species'!H14</f>
+        <v>8.1601999999999997</v>
+      </c>
+      <c r="E12" s="9">
+        <f>'AD table_species'!J14</f>
+        <v>14.378966670000001</v>
+      </c>
+      <c r="F12" s="9">
+        <f>'AD table_species'!L14</f>
+        <v>23.903416669999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC552C38-DABE-A944-89ED-E0BD7978AC5E}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="9">
+        <f>Sens!D4</f>
+        <v>36.363599999999998</v>
+      </c>
+      <c r="C2" s="9">
+        <f>Sens!F4</f>
+        <v>63.636400000000002</v>
+      </c>
+      <c r="D2" s="9">
+        <f>Sens!H4</f>
+        <v>54.545499999999997</v>
+      </c>
+      <c r="E2" s="9">
+        <f>Sens!J4</f>
+        <v>45.454500000000003</v>
+      </c>
+      <c r="F2" s="9">
+        <f>Sens!L4</f>
+        <v>9.0908999999999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="9">
+        <f>Sens!D5</f>
+        <v>100</v>
+      </c>
+      <c r="C3" s="9">
+        <f>Sens!F5</f>
+        <v>89.473699999999994</v>
+      </c>
+      <c r="D3" s="9">
+        <f>Sens!H5</f>
+        <v>97.368399999999994</v>
+      </c>
+      <c r="E3" s="9">
+        <f>Sens!J5</f>
+        <v>97.368399999999994</v>
+      </c>
+      <c r="F3" s="9">
+        <f>Sens!L5</f>
+        <v>86.842100000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="9">
+        <f>Sens!D6</f>
+        <v>100</v>
+      </c>
+      <c r="C4" s="9">
+        <f>Sens!F6</f>
+        <v>95.238100000000003</v>
+      </c>
+      <c r="D4" s="9">
+        <f>Sens!H6</f>
+        <v>100</v>
+      </c>
+      <c r="E4" s="9">
+        <f>Sens!J6</f>
+        <v>100</v>
+      </c>
+      <c r="F4" s="9">
+        <f>Sens!L6</f>
+        <v>80.952399999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9">
+        <f>Sens!D7</f>
+        <v>85.714299999999994</v>
+      </c>
+      <c r="C5" s="9">
+        <f>Sens!F7</f>
+        <v>92.857100000000003</v>
+      </c>
+      <c r="D5" s="9">
+        <f>Sens!H7</f>
+        <v>92.857100000000003</v>
+      </c>
+      <c r="E5" s="9">
+        <f>Sens!J7</f>
+        <v>100</v>
+      </c>
+      <c r="F5" s="9">
+        <f>Sens!L7</f>
+        <v>85.714299999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="9">
+        <f>Sens!D8</f>
+        <v>81.818200000000004</v>
+      </c>
+      <c r="C6" s="9">
+        <f>Sens!F8</f>
+        <v>90.909099999999995</v>
+      </c>
+      <c r="D6" s="9">
+        <f>Sens!H8</f>
+        <v>72.7273</v>
+      </c>
+      <c r="E6" s="9">
+        <f>Sens!J8</f>
+        <v>100</v>
+      </c>
+      <c r="F6" s="9">
+        <f>Sens!L8</f>
+        <v>90.909099999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="9">
+        <f>Sens!D9</f>
+        <v>72.7273</v>
+      </c>
+      <c r="C7" s="9">
+        <f>Sens!F9</f>
+        <v>72.7273</v>
+      </c>
+      <c r="D7" s="9">
+        <f>Sens!H9</f>
+        <v>81.818200000000004</v>
+      </c>
+      <c r="E7" s="9">
+        <f>Sens!J9</f>
+        <v>100</v>
+      </c>
+      <c r="F7" s="9">
+        <f>Sens!L9</f>
+        <v>90.909099999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="9">
+        <f>Sens!D10</f>
+        <v>63.636400000000002</v>
+      </c>
+      <c r="C8" s="9">
+        <f>Sens!F10</f>
+        <v>63.636400000000002</v>
+      </c>
+      <c r="D8" s="9">
+        <f>Sens!H10</f>
+        <v>90.909099999999995</v>
+      </c>
+      <c r="E8" s="9">
+        <f>Sens!J10</f>
+        <v>100</v>
+      </c>
+      <c r="F8" s="9">
+        <f>Sens!L10</f>
+        <v>81.818200000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="9">
+        <f>Sens!D11</f>
+        <v>72.7273</v>
+      </c>
+      <c r="C9" s="9">
+        <f>Sens!F11</f>
+        <v>72.7273</v>
+      </c>
+      <c r="D9" s="9">
+        <f>Sens!H11</f>
+        <v>81.818200000000004</v>
+      </c>
+      <c r="E9" s="9">
+        <f>Sens!J11</f>
+        <v>100</v>
+      </c>
+      <c r="F9" s="9">
+        <f>Sens!L11</f>
+        <v>81.818200000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="9">
+        <f>Sens!D12</f>
+        <v>89.473699999999994</v>
+      </c>
+      <c r="C10" s="9">
+        <f>Sens!F12</f>
+        <v>100</v>
+      </c>
+      <c r="D10" s="9">
+        <f>Sens!H12</f>
+        <v>98.947360000000003</v>
+      </c>
+      <c r="E10" s="9">
+        <f>Sens!J12</f>
+        <v>89.473699999999994</v>
+      </c>
+      <c r="F10" s="9">
+        <f>Sens!L12</f>
+        <v>94.736800000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="9">
+        <f>Sens!D13</f>
+        <v>94.736800000000002</v>
+      </c>
+      <c r="C11" s="9">
+        <f>Sens!F13</f>
+        <v>100</v>
+      </c>
+      <c r="D11" s="9">
+        <f>Sens!H13</f>
+        <v>100</v>
+      </c>
+      <c r="E11" s="9">
+        <f>Sens!J13</f>
+        <v>89.473699999999994</v>
+      </c>
+      <c r="F11" s="9">
+        <f>Sens!L13</f>
+        <v>94.736800000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="9">
+        <f>Sens!D14</f>
+        <v>78.947400000000002</v>
+      </c>
+      <c r="C12" s="9">
+        <f>Sens!F14</f>
+        <v>94.736800000000002</v>
+      </c>
+      <c r="D12" s="9">
+        <f>Sens!H14</f>
+        <v>100</v>
+      </c>
+      <c r="E12" s="9">
+        <f>Sens!J14</f>
+        <v>89.473699999999994</v>
+      </c>
+      <c r="F12" s="9">
+        <f>Sens!L14</f>
+        <v>94.736800000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="E2" formula="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{840725BD-5507-AF49-91E4-9B9A3EA7E0D9}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="9">
+        <f>FPRA!D4</f>
+        <v>2.6303000000000001</v>
+      </c>
+      <c r="C2" s="9">
+        <f>FPRA!F4</f>
+        <v>17.926600000000001</v>
+      </c>
+      <c r="D2" s="9">
+        <f>FPRA!H4</f>
+        <v>50.043799999999997</v>
+      </c>
+      <c r="E2" s="9">
+        <f>FPRA!J4</f>
+        <v>37.344299999999997</v>
+      </c>
+      <c r="F2" s="9">
+        <f>FPRA!L4</f>
+        <v>11.964700000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="9">
+        <f>FPRA!D5</f>
+        <v>0.52649999999999997</v>
+      </c>
+      <c r="C3" s="9">
+        <f>FPRA!F5</f>
+        <v>3.0566</v>
+      </c>
+      <c r="D3" s="9">
+        <f>FPRA!H5</f>
+        <v>1.4388000000000001</v>
+      </c>
+      <c r="E3" s="9">
+        <f>FPRA!J5</f>
+        <v>2.0432000000000001</v>
+      </c>
+      <c r="F3" s="9">
+        <f>FPRA!L5</f>
+        <v>8.5091000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="9">
+        <f>FPRA!D6</f>
+        <v>5.8599999999999999E-2</v>
+      </c>
+      <c r="C4" s="9">
+        <f>FPRA!F6</f>
+        <v>3.8344</v>
+      </c>
+      <c r="D4" s="9">
+        <f>FPRA!H6</f>
+        <v>0.20549999999999999</v>
+      </c>
+      <c r="E4" s="9">
+        <f>FPRA!J6</f>
+        <v>3.9102000000000001</v>
+      </c>
+      <c r="F4" s="9">
+        <f>FPRA!L6</f>
+        <v>30.666799999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9">
+        <f>FPRA!D7</f>
+        <v>2.6644999999999999</v>
+      </c>
+      <c r="C5" s="9">
+        <f>FPRA!F7</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="9">
+        <f>FPRA!H7</f>
+        <v>0.2104</v>
+      </c>
+      <c r="E5" s="9">
+        <f>FPRA!J7</f>
+        <v>1.1600999999999999</v>
+      </c>
+      <c r="F5" s="9">
+        <f>FPRA!L7</f>
+        <v>26.4802</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="9">
+        <f>FPRA!D8</f>
+        <v>0.84640000000000004</v>
+      </c>
+      <c r="C6" s="9">
+        <f>FPRA!F8</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="9">
+        <f>FPRA!H8</f>
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="E6" s="9">
+        <f>FPRA!J8</f>
+        <v>0.67810000000000004</v>
+      </c>
+      <c r="F6" s="9">
+        <f>FPRA!L8</f>
+        <v>30.915199999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="9">
+        <f>FPRA!D9</f>
+        <v>11.4154</v>
+      </c>
+      <c r="C7" s="9">
+        <f>FPRA!F9</f>
+        <v>1.41E-2</v>
+      </c>
+      <c r="D7" s="9">
+        <f>FPRA!H9</f>
+        <v>0.26550000000000001</v>
+      </c>
+      <c r="E7" s="9">
+        <f>FPRA!J9</f>
+        <v>1.0866</v>
+      </c>
+      <c r="F7" s="9">
+        <f>FPRA!L9</f>
+        <v>31.056799999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="9">
+        <f>FPRA!D10</f>
+        <v>32.056699999999999</v>
+      </c>
+      <c r="C8" s="9">
+        <f>FPRA!F10</f>
+        <v>32.309399999999997</v>
+      </c>
+      <c r="D8" s="9">
+        <f>FPRA!H10</f>
+        <v>22.333500000000001</v>
+      </c>
+      <c r="E8" s="9">
+        <f>FPRA!J10</f>
+        <v>9.1620000000000008</v>
+      </c>
+      <c r="F8" s="9">
+        <f>FPRA!L10</f>
+        <v>69.168199999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="9">
+        <f>FPRA!D11</f>
+        <v>6.0699999999999997E-2</v>
+      </c>
+      <c r="C9" s="9">
+        <f>FPRA!F11</f>
+        <v>0.1024</v>
+      </c>
+      <c r="D9" s="9">
+        <f>FPRA!H11</f>
+        <v>1.9400000000000001E-2</v>
+      </c>
+      <c r="E9" s="9">
+        <f>FPRA!J11</f>
+        <v>0.25059999999999999</v>
+      </c>
+      <c r="F9" s="9">
+        <f>FPRA!L11</f>
+        <v>13.194800000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="9">
+        <f>FPRA!D12</f>
+        <v>9.5399999999999999E-3</v>
+      </c>
+      <c r="C10" s="9">
+        <f>FPRA!F12</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="9">
+        <f>FPRA!H12</f>
+        <v>3.2694000000000001</v>
+      </c>
+      <c r="E10" s="9">
+        <f>FPRA!J12</f>
+        <v>4.06548</v>
+      </c>
+      <c r="F10" s="9">
+        <f>FPRA!L12</f>
+        <v>22.23968</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="9">
+        <f>FPRA!D13</f>
+        <v>3.86411999999999</v>
+      </c>
+      <c r="C11" s="9">
+        <f>FPRA!F13</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="9">
+        <f>FPRA!H13</f>
+        <v>9.7552800000000008</v>
+      </c>
+      <c r="E11" s="9">
+        <f>FPRA!J13</f>
+        <v>14.06352</v>
+      </c>
+      <c r="F11" s="9">
+        <f>FPRA!L13</f>
+        <v>27.3918</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="9">
+        <f>FPRA!D14</f>
+        <v>12.22505</v>
+      </c>
+      <c r="C12" s="9">
+        <f>FPRA!F14</f>
+        <v>4.7166166666666598</v>
+      </c>
+      <c r="D12" s="9">
+        <f>FPRA!H14</f>
+        <v>9.7893166666666591</v>
+      </c>
+      <c r="E12" s="9">
+        <f>FPRA!J14</f>
+        <v>20.190933333333302</v>
+      </c>
+      <c r="F12" s="9">
+        <f>FPRA!L14</f>
+        <v>26.144283333333298</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated heatmaps with replicates, added stdev to AD table
</commit_message>
<xml_diff>
--- a/utils/paper/ad_table.xlsx
+++ b/utils/paper/ad_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valenciaem/coding/pipelines/utils/paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3281259-FF5E-984A-A0A5-D5D261936F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3497D184-BAD2-DF4B-9C76-77D271E9FC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3420" yWindow="3500" windowWidth="23040" windowHeight="16900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -142,7 +142,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -266,6 +266,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -277,12 +283,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -594,7 +594,7 @@
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView zoomScale="111" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:N15"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -607,22 +607,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
     </row>
     <row r="2" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="10" t="s">
@@ -631,27 +631,27 @@
       <c r="C2" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16" t="s">
+      <c r="E2" s="20"/>
+      <c r="F2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16" t="s">
+      <c r="G2" s="20"/>
+      <c r="H2" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16" t="s">
+      <c r="I2" s="20"/>
+      <c r="J2" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16" t="s">
+      <c r="K2" s="20"/>
+      <c r="L2" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="16"/>
-      <c r="N2" s="22" t="s">
+      <c r="M2" s="20"/>
+      <c r="N2" s="18" t="s">
         <v>30</v>
       </c>
     </row>
@@ -688,7 +688,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="19" t="s">
         <v>16</v>
       </c>
       <c r="B4" t="s">
@@ -723,7 +723,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
+      <c r="A5" s="19"/>
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -751,12 +751,12 @@
       </c>
       <c r="M5" s="9"/>
       <c r="N5" s="9">
-        <f t="shared" ref="N5:N15" si="0">AVERAGE(D5,F5,H5,J5,L5)</f>
+        <f t="shared" ref="N5:N14" si="0">AVERAGE(D5,F5,H5,J5,L5)</f>
         <v>16.131119999999999</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="15"/>
+      <c r="A6" s="19"/>
       <c r="B6" t="s">
         <v>0</v>
       </c>
@@ -789,7 +789,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
+      <c r="A7" s="19"/>
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -822,7 +822,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
+      <c r="A8" s="19"/>
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -855,7 +855,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
+      <c r="A9" s="19"/>
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -888,7 +888,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="15"/>
+      <c r="A10" s="19"/>
       <c r="B10" t="s">
         <v>3</v>
       </c>
@@ -921,7 +921,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="15"/>
+      <c r="A11" s="19"/>
       <c r="B11" t="s">
         <v>6</v>
       </c>
@@ -954,7 +954,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="19" t="s">
         <v>17</v>
       </c>
       <c r="B12" t="s">
@@ -999,7 +999,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="15"/>
+      <c r="A13" s="19"/>
       <c r="B13" t="s">
         <v>21</v>
       </c>
@@ -1042,7 +1042,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="15"/>
+      <c r="A14" s="19"/>
       <c r="B14" t="s">
         <v>9</v>
       </c>
@@ -1088,33 +1088,49 @@
       <c r="A15" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="15" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="9">
         <f t="shared" ref="D15:L15" si="1">AVERAGE(D4:D14)</f>
         <v>9.9879948481818186</v>
       </c>
-      <c r="E15" s="9"/>
+      <c r="E15" s="9">
+        <f>STDEV(D4:D14)</f>
+        <v>4.6082827970238309</v>
+      </c>
       <c r="F15" s="9">
         <f t="shared" si="1"/>
         <v>6.9986572727272724</v>
       </c>
-      <c r="G15" s="9"/>
+      <c r="G15" s="9">
+        <f>STDEV(F4:F14)</f>
+        <v>4.044501631430232</v>
+      </c>
       <c r="H15" s="9">
         <f t="shared" si="1"/>
         <v>12.742581818181817</v>
       </c>
-      <c r="I15" s="9"/>
+      <c r="I15" s="9">
+        <f>STDEV(H4:H14)</f>
+        <v>4.5763867689211279</v>
+      </c>
       <c r="J15" s="9">
         <f t="shared" si="1"/>
         <v>12.757096970000003</v>
       </c>
-      <c r="K15" s="9"/>
+      <c r="K15" s="9">
+        <f>STDEV(J4:J14)</f>
+        <v>4.9130246311651584</v>
+      </c>
       <c r="L15" s="9">
         <f t="shared" si="1"/>
         <v>23.084812424545454</v>
       </c>
+      <c r="M15" s="9">
+        <f>STDEV(L4:L14)</f>
+        <v>3.8673744569811461</v>
+      </c>
       <c r="N15" s="9"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -1125,14 +1141,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="A1:N1"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A4:A11"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="A1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1144,7 +1160,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView zoomScale="118" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1156,22 +1172,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -1181,26 +1197,26 @@
       <c r="C2" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18" t="s">
+      <c r="E2" s="22"/>
+      <c r="F2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18" t="s">
+      <c r="G2" s="22"/>
+      <c r="H2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18" t="s">
+      <c r="I2" s="22"/>
+      <c r="J2" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18" t="s">
+      <c r="K2" s="22"/>
+      <c r="L2" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="18"/>
+      <c r="M2" s="22"/>
       <c r="N2" s="10" t="s">
         <v>30</v>
       </c>
@@ -1242,7 +1258,7 @@
       <c r="N3" s="7"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="21" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1275,10 +1291,10 @@
         <f>AVERAGE(D4,F4,H4,J4,L4)</f>
         <v>41.818179999999998</v>
       </c>
-      <c r="O4" s="20"/>
+      <c r="O4" s="16"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="17"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1309,10 +1325,10 @@
         <f t="shared" ref="N5:N14" si="0">AVERAGE(D5,F5,H5,J5,L5)</f>
         <v>94.210520000000002</v>
       </c>
-      <c r="O5" s="20"/>
+      <c r="O5" s="16"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="17"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1343,10 +1359,10 @@
         <f t="shared" si="0"/>
         <v>95.238100000000003</v>
       </c>
-      <c r="O6" s="20"/>
+      <c r="O6" s="16"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="17"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
@@ -1377,10 +1393,10 @@
         <f t="shared" si="0"/>
         <v>91.42855999999999</v>
       </c>
-      <c r="O7" s="20"/>
+      <c r="O7" s="16"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="17"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
@@ -1411,10 +1427,10 @@
         <f t="shared" si="0"/>
         <v>87.272739999999999</v>
       </c>
-      <c r="O8" s="20"/>
+      <c r="O8" s="16"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="17"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
@@ -1445,10 +1461,10 @@
         <f t="shared" si="0"/>
         <v>83.636380000000003</v>
       </c>
-      <c r="O9" s="20"/>
+      <c r="O9" s="16"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="17"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="3" t="s">
         <v>3</v>
       </c>
@@ -1479,10 +1495,10 @@
         <f t="shared" si="0"/>
         <v>80.000019999999992</v>
       </c>
-      <c r="O10" s="20"/>
+      <c r="O10" s="16"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="3" t="s">
         <v>6</v>
       </c>
@@ -1513,10 +1529,10 @@
         <f t="shared" si="0"/>
         <v>81.818200000000004</v>
       </c>
-      <c r="O11" s="20"/>
+      <c r="O11" s="16"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="21" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1559,10 +1575,10 @@
         <f t="shared" si="0"/>
         <v>94.526312000000004</v>
       </c>
-      <c r="O12" s="20"/>
+      <c r="O12" s="16"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="17"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="3" t="s">
         <v>21</v>
       </c>
@@ -1603,10 +1619,10 @@
         <f t="shared" si="0"/>
         <v>95.789460000000005</v>
       </c>
-      <c r="O13" s="20"/>
+      <c r="O13" s="16"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="17"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="3" t="s">
         <v>9</v>
       </c>
@@ -1647,7 +1663,7 @@
         <f t="shared" si="0"/>
         <v>91.578940000000017</v>
       </c>
-      <c r="O14" s="20"/>
+      <c r="O14" s="16"/>
     </row>
     <row r="15" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
@@ -1656,31 +1672,45 @@
       <c r="B15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="17">
         <f>AVERAGE(D4:D14)</f>
         <v>79.649545454545461</v>
       </c>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21">
+      <c r="E15" s="4">
+        <v>18.489999999999998</v>
+      </c>
+      <c r="F15" s="17">
         <f>AVERAGE(F4:F14)</f>
         <v>85.085654545454545</v>
       </c>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21">
+      <c r="G15" s="9">
+        <f>STDEV(F4:F14)</f>
+        <v>14.072149365137026</v>
+      </c>
+      <c r="H15" s="17">
         <f>AVERAGE(H4:H14)</f>
         <v>88.271923636363638</v>
       </c>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21">
+      <c r="I15" s="9">
+        <f>STDEV(H4:H14)</f>
+        <v>14.490482268252631</v>
+      </c>
+      <c r="J15" s="17">
         <f>AVERAGE(J4:J14)</f>
         <v>91.931272727272727</v>
       </c>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21">
+      <c r="K15" s="9">
+        <f>STDEV(J4:J14)</f>
+        <v>16.119546848661191</v>
+      </c>
+      <c r="L15" s="17">
         <f>AVERAGE(L4:L14)</f>
         <v>81.114972727272729</v>
       </c>
-      <c r="M15" s="9"/>
+      <c r="M15" s="9">
+        <f>STDEV(L4:L14)</f>
+        <v>24.476414627722338</v>
+      </c>
       <c r="N15" s="9"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
@@ -1691,14 +1721,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="A1:N1"/>
     <mergeCell ref="A4:A11"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="A1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1709,7 +1739,7 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1720,22 +1750,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -1745,26 +1775,26 @@
       <c r="C2" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18" t="s">
+      <c r="E2" s="22"/>
+      <c r="F2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18" t="s">
+      <c r="G2" s="22"/>
+      <c r="H2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18" t="s">
+      <c r="I2" s="22"/>
+      <c r="J2" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18" t="s">
+      <c r="K2" s="22"/>
+      <c r="L2" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="18"/>
+      <c r="M2" s="22"/>
       <c r="N2" s="10" t="s">
         <v>30</v>
       </c>
@@ -1805,7 +1835,7 @@
       <c r="N3" s="7"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="21" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1840,7 +1870,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="17"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1873,7 +1903,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="17"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1906,7 +1936,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="17"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
@@ -1939,7 +1969,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="17"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
@@ -1972,7 +2002,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="17"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
@@ -2005,7 +2035,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="17"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="3" t="s">
         <v>3</v>
       </c>
@@ -2038,7 +2068,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="3" t="s">
         <v>6</v>
       </c>
@@ -2071,7 +2101,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="21" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -2116,7 +2146,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="17"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="3" t="s">
         <v>21</v>
       </c>
@@ -2159,7 +2189,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="17"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="3" t="s">
         <v>9</v>
       </c>
@@ -2212,37 +2242,53 @@
         <f>AVERAGE(D4:D14)</f>
         <v>6.0325281818181802</v>
       </c>
-      <c r="E15" s="9"/>
+      <c r="E15" s="9">
+        <f>STDEV(D4:D14)</f>
+        <v>9.6800833004151556</v>
+      </c>
       <c r="F15" s="9">
         <f t="shared" ref="F15:L15" si="1">AVERAGE(F4:F14)</f>
         <v>5.6327378787878777</v>
       </c>
-      <c r="G15" s="9"/>
+      <c r="G15" s="9">
+        <f>STDEV(F4:F14)</f>
+        <v>10.308044451145078</v>
+      </c>
       <c r="H15" s="9">
         <f t="shared" si="1"/>
         <v>8.8529906060606063</v>
       </c>
-      <c r="I15" s="9"/>
+      <c r="I15" s="9">
+        <f>STDEV(H4:H14)</f>
+        <v>15.313238295042975</v>
+      </c>
       <c r="J15" s="9">
         <f t="shared" si="1"/>
         <v>8.5413666666666632</v>
       </c>
-      <c r="K15" s="9"/>
+      <c r="K15" s="9">
+        <f>STDEV(J4:J14)</f>
+        <v>11.491442858592743</v>
+      </c>
       <c r="L15" s="9">
         <f t="shared" si="1"/>
         <v>27.066505757575758</v>
       </c>
+      <c r="M15" s="9">
+        <f>STDEV(L4:L14)</f>
+        <v>16.142224290110438</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="A1:N1"/>
     <mergeCell ref="A4:A11"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="A1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>